<commit_message>
creat account with personal data test added
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="Credentials" sheetId="2" r:id="rId2"/>
-    <sheet name="Email" sheetId="3" r:id="rId3"/>
-    <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
-    <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
-    <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="2" r:id="rId4"/>
+    <sheet name="Email" sheetId="3" r:id="rId5"/>
+    <sheet name="ProductDetails" sheetId="4" r:id="rId6"/>
+    <sheet name="SearchProduct" sheetId="6" r:id="rId7"/>
+    <sheet name="AccountCreationData" sheetId="7" r:id="rId8"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>TestCases</t>
   </si>
@@ -288,25 +289,25 @@
   </si>
   <si>
     <t>newtest1@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest2@gmail.com</t>
-  </si>
-  <si>
-    <t>newtest3@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -317,7 +318,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -333,13 +334,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.5999900102615356"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,78 +355,95 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
+      <alignment/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -435,34 +453,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="20" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="20" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -750,30 +857,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{aa138fff-fac2-4de6-a743-f8ffe00edd85}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0" topLeftCell="A4">
+      <selection pane="topLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.142857142857142" customWidth="1"/>
+    <col min="2" max="2" width="23.714285714285715" customWidth="1"/>
+    <col min="3" max="4" width="26.285714285714285" customWidth="1"/>
+    <col min="5" max="5" width="44.42857142857143" customWidth="1"/>
+    <col min="6" max="6" width="20.571428571428573" customWidth="1"/>
+    <col min="7" max="7" width="22.714285714285715" customWidth="1"/>
+    <col min="8" max="8" width="17.142857142857142" customWidth="1"/>
+    <col min="9" max="9" width="18.714285714285715" customWidth="1"/>
+    <col min="10" max="10" width="23.428571428571427" customWidth="1"/>
+    <col min="11" max="11" width="15.714285714285714" customWidth="1"/>
+    <col min="12" max="12" width="17.571428571428573" customWidth="1"/>
+    <col min="13" max="13" width="20.857142857142858" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
@@ -781,7 +888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -789,7 +896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:2" ht="15">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
@@ -797,7 +904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="13" t="s">
         <v>38</v>
       </c>
@@ -806,7 +913,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -823,7 +930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -840,7 +947,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -857,7 +964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -874,7 +981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -891,7 +998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -908,7 +1015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -930,7 +1037,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -945,7 +1052,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -956,7 +1063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -965,7 +1072,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -974,7 +1081,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -983,7 +1090,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1005,28 +1112,28 @@
     <mergeCell ref="A4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="1" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6db8c93e-34b6-4a4c-9b55-bdbf59713848}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.714285714285714" customWidth="1"/>
+    <col min="2" max="2" width="12.285714285714286" customWidth="1"/>
+    <col min="3" max="3" width="13.571428571428571" customWidth="1"/>
+    <col min="4" max="4" width="17.714285714285715" customWidth="1"/>
+    <col min="5" max="5" width="17.285714285714285" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
@@ -1034,7 +1141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" s="9" t="s">
         <v>50</v>
       </c>
@@ -1044,55 +1151,55 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" display="admin@xyz.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId3"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="1" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753a029f-2e86-4a3f-93e3-8a74e7974daf}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.571428571428573" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="10" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="ghfsdtyfg@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="1" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3513cd0d-6ce5-4c4e-af77-c55d620a4846}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A1" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
@@ -1103,7 +1210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -1120,19 +1227,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e38adba6-7b07-427c-bb09-48a910164f01}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -1143,33 +1250,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e6b48832-84af-44db-b22b-63e317ea25ab}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.714285714285714" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.714285714285714" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.285714285714286" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.285714285714286" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.285714285714286" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.571428571428571" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.428571428571429" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.714285714285714" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.857142857142858" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.285714285714286" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="8" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1323,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15">
       <c r="A2" s="11" t="s">
         <v>87</v>
       </c>
@@ -1263,105 +1370,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" display="newtest1@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>